<commit_message>
Updated BOM for Revision B
</commit_message>
<xml_diff>
--- a/LED Driver BOM.xlsx
+++ b/LED Driver BOM.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\innolab\Documents\eagle\Engineering Brightness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\innolab\Documents\eagle\Engineering-Brightness\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rev A" sheetId="1" r:id="rId1"/>
+    <sheet name="Rev B" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>Part</t>
   </si>
@@ -150,14 +151,130 @@
   </si>
   <si>
     <t>RC0603JR-0791KL</t>
+  </si>
+  <si>
+    <t>240k</t>
+  </si>
+  <si>
+    <t>RMCF0603JT240KCT-ND</t>
+  </si>
+  <si>
+    <t>240k Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603JT240K</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Cost per Board</t>
+  </si>
+  <si>
+    <t>Quantity per Board</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>JST-RCY-Female</t>
+  </si>
+  <si>
+    <t>JST-RCY-Male</t>
+  </si>
+  <si>
+    <t>Onboard:</t>
+  </si>
+  <si>
+    <t>Offboard:</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>eBoot 20 AWG JST Plug Connector 2 Pin Male Female Plug Connector Cable Wire for LED Lamp Strip RC Toys Battery, 10 Pairs</t>
+  </si>
+  <si>
+    <t>PTH</t>
+  </si>
+  <si>
+    <t>Power Input Connector</t>
+  </si>
+  <si>
+    <t>Power Output Connector</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Panel Mount</t>
+  </si>
+  <si>
+    <t>Dimming Potentiometer</t>
+  </si>
+  <si>
+    <t>JST-SM-Female</t>
+  </si>
+  <si>
+    <t>JST-SM-Male</t>
+  </si>
+  <si>
+    <t>HKBAYI 50Pair / 50sets 3 pin JST SM Male Female plug LED Connector Cable For WS2812B WS2812 WS2811 LED Strip Lamp with 15cm Long Wire</t>
+  </si>
+  <si>
+    <t>Dimming Pot Connector</t>
+  </si>
+  <si>
+    <t>All Unit Costs evaluated at a quantity of 25</t>
+  </si>
+  <si>
+    <t>987-1394-ND</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>P110KV1-1F15BR100K</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Total Cost per Board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -173,7 +290,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -181,13 +298,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,4 +828,514 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <f>G3*H3</f>
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1206</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.2424</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" ref="I4:I12" si="0">G4*H4</f>
+        <v>0.2424</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.16225000000000001</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.16225000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.16225000000000001</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.16225000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6">
+        <f>G16*H16</f>
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6">
+        <f>G17*H17</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6">
+        <f>G19*H19</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="8">
+        <f>SUM(I3:I12,I16:I19)</f>
+        <v>4.6219000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A14:K14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated LED Driver BOM
Forgot that the output connector is supplied by RapidLED
</commit_message>
<xml_diff>
--- a/LED Driver BOM.xlsx
+++ b/LED Driver BOM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
   <si>
     <t>Part</t>
   </si>
@@ -192,9 +192,6 @@
     <t>JST-RCY-Female</t>
   </si>
   <si>
-    <t>JST-RCY-Male</t>
-  </si>
-  <si>
     <t>Onboard:</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Power Output Connector</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Panel Mount</t>
   </si>
   <si>
@@ -256,6 +250,15 @@
   </si>
   <si>
     <t>Total Cost per Board</t>
+  </si>
+  <si>
+    <t>(PCBway)</t>
+  </si>
+  <si>
+    <t>(Amazon)</t>
+  </si>
+  <si>
+    <t>(RapidLED)</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -332,16 +335,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,7 +838,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,25 +848,25 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="A1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -875,7 +878,7 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -884,13 +887,13 @@
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -919,13 +922,13 @@
       <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>0.77400000000000002</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <f>G3*H3</f>
         <v>0.77400000000000002</v>
       </c>
@@ -949,13 +952,13 @@
       <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.2424</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <f t="shared" ref="I4:I12" si="0">G4*H4</f>
         <v>0.2424</v>
       </c>
@@ -979,13 +982,13 @@
       <c r="F5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f t="shared" si="0"/>
         <v>1.2999999999999999E-2</v>
       </c>
@@ -1009,13 +1012,13 @@
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1039,13 +1042,13 @@
       <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>0.03</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
@@ -1066,13 +1069,13 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0.81299999999999994</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <f t="shared" si="0"/>
         <v>0.81299999999999994</v>
       </c>
@@ -1093,13 +1096,13 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>0.77400000000000002</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <f t="shared" si="0"/>
         <v>0.77400000000000002</v>
       </c>
@@ -1112,24 +1115,24 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" t="s">
         <v>61</v>
       </c>
-      <c r="E10" t="s">
-        <v>62</v>
-      </c>
       <c r="F10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="6">
+        <v>76</v>
+      </c>
+      <c r="G10" s="5">
         <v>0.16225000000000001</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <f t="shared" si="0"/>
         <v>0.16225000000000001</v>
       </c>
@@ -1138,30 +1141,17 @@
       <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.16225000000000001</v>
+        <v>77</v>
       </c>
       <c r="H11">
         <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <f t="shared" si="0"/>
-        <v>0.16225000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1169,45 +1159,45 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
         <v>67</v>
       </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="6">
+        <v>76</v>
+      </c>
+      <c r="G12" s="5">
         <v>0.12</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="A14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1219,7 +1209,7 @@
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1228,13 +1218,13 @@
       <c r="F15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>46</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J15" s="2" t="s">
@@ -1246,89 +1236,92 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="6">
+        <v>70</v>
+      </c>
+      <c r="G16" s="5">
         <v>0.75600000000000001</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <f>G16*H16</f>
         <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" t="s">
-        <v>70</v>
-      </c>
       <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="6">
+        <v>76</v>
+      </c>
+      <c r="G17" s="5">
         <v>0.12</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <f>G17*H17</f>
         <v>0.12</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>0.64</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <f>G19*H19</f>
         <v>0.64</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="8">
+        <v>69</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="7">
         <f>SUM(I3:I12,I16:I19)</f>
-        <v>4.6219000000000001</v>
+        <v>4.4596499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>